<commit_message>
1. 加上 LoadCell 資料 Read Command 2. 更新 程序 1, 1+2 顯示動畫
</commit_message>
<xml_diff>
--- a/Doc/ActTbl_Cmd.xlsx
+++ b/Doc/ActTbl_Cmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\621\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LoadingMachine\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8764BA43-1237-4B66-B4F4-01E6E457144C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7507956C-56F7-4581-9C50-7A286F044088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="497" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="497" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="621 Command" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="675">
   <si>
     <t>MOVE_X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3846,6 +3846,22 @@
   </si>
   <si>
     <t>■-探針失敗後執行 File No = 0xFFFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoadCell 資料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defUART_LoadCellData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Byte0~7 (Byte 0-1 Cell 0/Byte 2-3 Cell 1/Byte 4-5 Cell 2/Byte 6-7 Cell 3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4973,8 +4989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5745,6 +5761,26 @@
       </c>
       <c r="H36" s="84" t="s">
         <v>460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="B37" s="87" t="s">
+        <v>671</v>
+      </c>
+      <c r="E37" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="95" t="s">
+        <v>672</v>
+      </c>
+      <c r="G37" s="87" t="s">
+        <v>673</v>
+      </c>
+      <c r="H37" s="84" t="s">
+        <v>460</v>
+      </c>
+      <c r="I37" s="91" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="39" spans="1:19">

</xml_diff>

<commit_message>
Track large file using Git LFS
</commit_message>
<xml_diff>
--- a/Doc/ActTbl_Cmd.xlsx
+++ b/Doc/ActTbl_Cmd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LoadingMachine\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7507956C-56F7-4581-9C50-7A286F044088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB4360-009D-4B7E-AD8B-93309F9DCAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="497" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4990,7 +4990,7 @@
   <dimension ref="A1:AA106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>